<commit_message>
feat: Cambios en el codigo, reports y UML avanzado
</commit_message>
<xml_diff>
--- a/reports/Tiempo estimado-real.xlsx
+++ b/reports/Tiempo estimado-real.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismae\Documents\Universidad de Sevilla\DISEÑO Y PRUEBAS II\Workspace-24\Projects\Acme-SF-D01\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace-24\Projects\Acme-SF-D01\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464FF81F-81DB-4168-B1E6-67907D3658E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B342A8C6-8B2B-4A8B-BF06-10E675BEC4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="20">
   <si>
     <t>Rol</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Coste/hora</t>
+  </si>
+  <si>
+    <t>Tiempo estimado D02</t>
+  </si>
+  <si>
+    <t>Tiempo real D02</t>
   </si>
 </sst>
 </file>
@@ -1581,6 +1587,9 @@
                 <c:pt idx="1">
                   <c:v>38</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1651,6 +1660,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1681,6 +1693,36 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1746,6 +1788,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>minuros</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> dedicatos</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5295,7 +5397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9AF520-1A94-4357-9CE4-04F00D982623}">
   <dimension ref="B4:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -5553,10 +5655,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12886396-CDAF-4037-9656-80B26E0CDA1B}">
-  <dimension ref="B2:T21"/>
+  <dimension ref="B2:T37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5607,7 +5709,9 @@
       <c r="Q4" s="11">
         <v>38</v>
       </c>
-      <c r="R4" s="11"/>
+      <c r="R4" s="11">
+        <v>300</v>
+      </c>
       <c r="S4" s="11"/>
       <c r="T4" s="12"/>
     </row>
@@ -5621,7 +5725,9 @@
       <c r="Q5" s="9">
         <v>70</v>
       </c>
-      <c r="R5" s="9"/>
+      <c r="R5" s="9">
+        <v>540</v>
+      </c>
       <c r="S5" s="9"/>
       <c r="T5" s="10"/>
     </row>
@@ -5711,26 +5817,138 @@
       </c>
       <c r="L10" s="46"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="G31" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="40"/>
+      <c r="D33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="41"/>
+      <c r="I33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="50"/>
+      <c r="D34" s="4">
+        <v>30</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="50"/>
+      <c r="I34" s="4">
+        <v>30</v>
+      </c>
+      <c r="J34" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="50"/>
+      <c r="D35" s="4">
+        <v>20</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+      <c r="G35" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="50"/>
+      <c r="I35" s="4">
+        <v>20</v>
+      </c>
+      <c r="J35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="44"/>
+      <c r="D37" s="47">
+        <f>D34*E34 + D35*E35</f>
+        <v>120</v>
+      </c>
+      <c r="E37" s="47"/>
+      <c r="G37" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="46"/>
+      <c r="I37" s="48">
+        <f>I34*J34+I35*J35</f>
+        <v>220</v>
+      </c>
+      <c r="J37" s="46"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="24">
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="I10:J10"/>

</xml_diff>

<commit_message>
- Documentacion y reordenacion por entregable
Signed-off-by: IsmaelGata <isgatdor@alum.us.es>
</commit_message>
<xml_diff>
--- a/reports/Tiempo estimado-real.xlsx
+++ b/reports/Tiempo estimado-real.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismae\Documents\Universidad de Sevilla\DISEÑO Y PRUEBAS II\Workspace-24\Projects\Acme-SF-D01\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismae\Documents\Universidad de Sevilla\DISEÑO Y PRUEBAS II\Workspace-24\Projects\Acme-SF-D02\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464FF81F-81DB-4168-B1E6-67907D3658E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8FBBC2-6437-4A2A-859A-DE13C1DD9191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="20">
   <si>
     <t>Rol</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Coste/hora</t>
+  </si>
+  <si>
+    <t>Tiempo estimado D2</t>
+  </si>
+  <si>
+    <t>Tiempo real D02</t>
   </si>
 </sst>
 </file>
@@ -1525,6 +1531,425 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'Hoja de Ismael'!$R$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimado (min)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Hoja de Ismael'!$S$15:$W$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Inicio</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>D01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>D02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>D04</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja de Ismael'!$S$16:$W$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7810-4A16-B973-00DC911D4C49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hoja de Ismael'!$R$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real (min)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Hoja de Ismael'!$S$15:$W$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Inicio</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>D01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>D02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>D04</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja de Ismael'!$S$17:$W$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7810-4A16-B973-00DC911D4C49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1845646639"/>
+        <c:axId val="2008140767"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1845646639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2008140767"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2008140767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1845646639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Tiempo de tareas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'Hoja de Juanjo'!$O$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1864,7 +2289,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -2443,6 +2868,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3992,6 +4457,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4585,6 +5566,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>863598</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>176741</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>106890</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>98424</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D13BF1D1-B498-40CB-9260-47480AB71EE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5293,10 +6312,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9AF520-1A94-4357-9CE4-04F00D982623}">
-  <dimension ref="B4:L21"/>
+  <dimension ref="B4:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5312,7 +6331,7 @@
     <col min="16" max="16" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>6</v>
       </c>
@@ -5327,8 +6346,22 @@
       <c r="J4" s="38"/>
       <c r="K4" s="38"/>
       <c r="L4" s="39"/>
+      <c r="O4" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="U4" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="39"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
         <v>0</v>
       </c>
@@ -5355,8 +6388,34 @@
       <c r="L6" s="24" t="s">
         <v>16</v>
       </c>
+      <c r="O6" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="U6" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" s="41"/>
+      <c r="W6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="24" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="42" t="s">
         <v>2</v>
       </c>
@@ -5385,8 +6444,36 @@
         <f>K7/60</f>
         <v>4.6333333333333337</v>
       </c>
+      <c r="O7" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="23">
+        <v>30</v>
+      </c>
+      <c r="R7" s="1">
+        <v>210</v>
+      </c>
+      <c r="S7" s="21">
+        <f>R7/60</f>
+        <v>3.5</v>
+      </c>
+      <c r="U7" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7" s="43"/>
+      <c r="W7" s="25">
+        <v>30</v>
+      </c>
+      <c r="X7" s="1">
+        <v>165</v>
+      </c>
+      <c r="Y7" s="26">
+        <f>X7/60</f>
+        <v>2.75</v>
+      </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8" s="42" t="s">
         <v>3</v>
       </c>
@@ -5416,8 +6503,37 @@
         <f>K8/60</f>
         <v>3.3166666666666669</v>
       </c>
+      <c r="O8" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="23">
+        <v>20</v>
+      </c>
+      <c r="R8" s="1">
+        <f>910</f>
+        <v>910</v>
+      </c>
+      <c r="S8" s="22">
+        <f>R8/60</f>
+        <v>15.166666666666666</v>
+      </c>
+      <c r="U8" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="V8" s="43"/>
+      <c r="W8" s="25">
+        <v>20</v>
+      </c>
+      <c r="X8" s="1">
+        <v>859</v>
+      </c>
+      <c r="Y8" s="27">
+        <f>X8/60</f>
+        <v>14.316666666666666</v>
+      </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" s="44" t="s">
         <v>5</v>
       </c>
@@ -5438,9 +6554,29 @@
       </c>
       <c r="K10" s="35"/>
       <c r="L10" s="35"/>
+      <c r="O10" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="45">
+        <f>Q7*S7+Q8*S8</f>
+        <v>408.33333333333331</v>
+      </c>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="U10" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="V10" s="46"/>
+      <c r="W10" s="35">
+        <f>W7*Y7+W8*Y8</f>
+        <v>368.83333333333331</v>
+      </c>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="35"/>
     </row>
-    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="15" t="s">
         <v>14</v>
       </c>
@@ -5457,7 +6593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E15" s="19" t="s">
         <v>8</v>
       </c>
@@ -5471,8 +6607,23 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="12"/>
+      <c r="S15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="U15" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="V15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="W15" s="17" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E16" s="18" t="s">
         <v>9</v>
       </c>
@@ -5486,27 +6637,72 @@
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="10"/>
+      <c r="R16" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="S16" s="13">
+        <v>0</v>
+      </c>
+      <c r="T16" s="11">
+        <f>R7+R8</f>
+        <v>1120</v>
+      </c>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="12"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S17" s="14">
+        <v>0</v>
+      </c>
+      <c r="T17" s="9">
+        <f>X7+X8</f>
+        <v>1024</v>
+      </c>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
+      <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="R22" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="24">
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:Y10"/>
+    <mergeCell ref="O4:S4"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:S10"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5525,6 +6721,26 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D1052085-6991-49A6-BC4A-2C23C8FC229A}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Hoja de Ismael'!T16:T16</xm:f>
+              <xm:sqref>U16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Hoja de Ismael'!T17:T17</xm:f>
+              <xm:sqref>U17</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{2F3E4048-3B25-4C64-BD72-4657033FB303}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>

</xml_diff>

<commit_message>
documentos grupales jimmy terminados
</commit_message>
<xml_diff>
--- a/reports/Tiempo estimado-real.xlsx
+++ b/reports/Tiempo estimado-real.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismae\Documents\Universidad de Sevilla\DISEÑO Y PRUEBAS II\Workspace-24\Projects\Acme-SF-D02\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DP2\Documents\Workspace-24\Projects\Acme-SF-D02\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A41A43-BDDF-4EDC-8E58-21AF43E40A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F55507-C170-41C1-B24B-E9615F4D6889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="4" r:id="rId1"/>
@@ -529,17 +529,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,6 +656,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.37588078912490541"/>
+          <c:y val="5.5595159483352266E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -750,7 +758,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -821,7 +829,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4532,15 +4540,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>730248</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>718342</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>110066</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>687915</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>902228</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>31749</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4997,8 +5005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D12626D-61D9-4105-9316-5A3F0038A1E8}">
   <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5055,7 +5063,7 @@
       </c>
       <c r="Q4" s="11">
         <f>E7+E8</f>
-        <v>110</v>
+        <v>455</v>
       </c>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
@@ -5070,7 +5078,7 @@
       </c>
       <c r="Q5" s="9">
         <f>K7+K8</f>
-        <v>140</v>
+        <v>789</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
@@ -5113,11 +5121,11 @@
         <v>30</v>
       </c>
       <c r="E7" s="1">
-        <v>45</v>
+        <v>275</v>
       </c>
       <c r="F7" s="21">
         <f>E7/60</f>
-        <v>0.75</v>
+        <v>4.583333333333333</v>
       </c>
       <c r="H7" s="43" t="s">
         <v>2</v>
@@ -5127,11 +5135,11 @@
         <v>30</v>
       </c>
       <c r="K7" s="1">
-        <v>90</v>
+        <v>361</v>
       </c>
       <c r="L7" s="26">
         <f>K7/60</f>
-        <v>1.5</v>
+        <v>6.0166666666666666</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -5143,12 +5151,11 @@
         <v>20</v>
       </c>
       <c r="E8" s="1">
-        <f>45+20</f>
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="F8" s="22">
         <f>E8/60</f>
-        <v>1.0833333333333333</v>
+        <v>3</v>
       </c>
       <c r="H8" s="43" t="s">
         <v>3</v>
@@ -5158,11 +5165,11 @@
         <v>20</v>
       </c>
       <c r="K8" s="1">
-        <v>50</v>
+        <v>428</v>
       </c>
       <c r="L8" s="27">
         <f>K8/60</f>
-        <v>0.83333333333333337</v>
+        <v>7.1333333333333337</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -5172,7 +5179,7 @@
       <c r="C10" s="44"/>
       <c r="D10" s="45">
         <f>D7*F7+D8*F8</f>
-        <v>44.166666666666664</v>
+        <v>197.5</v>
       </c>
       <c r="E10" s="45"/>
       <c r="F10" s="45"/>
@@ -5182,7 +5189,7 @@
       <c r="I10" s="46"/>
       <c r="J10" s="35">
         <f>J7*L7+J8*L8</f>
-        <v>61.666666666666671</v>
+        <v>323.16666666666669</v>
       </c>
       <c r="K10" s="35"/>
       <c r="L10" s="35"/>
@@ -5255,7 +5262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9AF520-1A94-4357-9CE4-04F00D982623}">
   <dimension ref="B4:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
@@ -5601,6 +5608,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5613,18 +5632,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5692,12 +5699,12 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
       <c r="I4" s="51" t="s">
         <v>7</v>
       </c>
@@ -5758,20 +5765,20 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="50"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="4">
         <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="50"/>
+      <c r="J7" s="48"/>
       <c r="K7" s="4">
         <v>30</v>
       </c>
@@ -5780,20 +5787,20 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="50"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="4">
         <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="50"/>
+      <c r="J8" s="48"/>
       <c r="K8" s="4">
         <v>20</v>
       </c>
@@ -5806,28 +5813,28 @@
         <v>5</v>
       </c>
       <c r="C10" s="44"/>
-      <c r="D10" s="47">
+      <c r="D10" s="49">
         <f>D7*E7 + D8*E8</f>
         <v>37.4</v>
       </c>
-      <c r="E10" s="47"/>
+      <c r="E10" s="49"/>
       <c r="I10" s="46" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="46"/>
-      <c r="K10" s="48">
+      <c r="K10" s="47">
         <f>K7*L7+K8*L8</f>
         <v>71.400000000000006</v>
       </c>
       <c r="L10" s="46"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
       <c r="I13" s="51" t="s">
         <v>19</v>
       </c>
@@ -5858,20 +5865,20 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="50"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="4">
         <v>30</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="I16" s="50" t="s">
+      <c r="I16" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="50"/>
+      <c r="J16" s="48"/>
       <c r="K16" s="4">
         <v>30</v>
       </c>
@@ -5880,20 +5887,20 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="4">
         <v>20</v>
       </c>
       <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="I17" s="50" t="s">
+      <c r="I17" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="50"/>
+      <c r="J17" s="48"/>
       <c r="K17" s="4">
         <v>20</v>
       </c>
@@ -5906,16 +5913,16 @@
         <v>5</v>
       </c>
       <c r="C19" s="44"/>
-      <c r="D19" s="47">
+      <c r="D19" s="49">
         <f>D16*E16 + D17*E17</f>
         <v>120</v>
       </c>
-      <c r="E19" s="47"/>
+      <c r="E19" s="49"/>
       <c r="I19" s="46" t="s">
         <v>5</v>
       </c>
       <c r="J19" s="46"/>
-      <c r="K19" s="48">
+      <c r="K19" s="47">
         <f>K16*L16+K17*L17</f>
         <v>220</v>
       </c>
@@ -5935,18 +5942,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="I16:J16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="I10:J10"/>
@@ -5959,6 +5954,18 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Añadido tiempo real de grupo
Signed-off-by: IsmaelGata <isgatdor@alum.us.es>
</commit_message>
<xml_diff>
--- a/reports/Tiempo estimado-real.xlsx
+++ b/reports/Tiempo estimado-real.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DP2\Documents\Workspace-24\Projects\Acme-SF-D02\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismae\Documents\Universidad de Sevilla\DISEÑO Y PRUEBAS II\Workspace-24\Projects\Acme-SF-D02\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F55507-C170-41C1-B24B-E9615F4D6889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FE6D9F-9D49-48B0-AC6B-061D346A3FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15990" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="21">
   <si>
     <t>Rol</t>
   </si>
@@ -529,17 +529,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -760,6 +760,9 @@
                 <c:pt idx="1">
                   <c:v>455</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>465</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -830,6 +833,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>723</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4540,16 +4546,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>718342</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>110066</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>51592</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>129116</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>902228</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>31749</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>6878</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5005,8 +5011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D12626D-61D9-4105-9316-5A3F0038A1E8}">
   <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5065,7 +5071,10 @@
         <f>E7+E8</f>
         <v>455</v>
       </c>
-      <c r="R4" s="11"/>
+      <c r="R4" s="11">
+        <f>E15+E16</f>
+        <v>465</v>
+      </c>
       <c r="S4" s="11"/>
       <c r="T4" s="12"/>
     </row>
@@ -5080,7 +5089,10 @@
         <f>K7+K8</f>
         <v>789</v>
       </c>
-      <c r="R5" s="9"/>
+      <c r="R5" s="9">
+        <f>K15+K16</f>
+        <v>723</v>
+      </c>
       <c r="S5" s="9"/>
       <c r="T5" s="10"/>
     </row>
@@ -5194,26 +5206,164 @@
       <c r="K10" s="35"/>
       <c r="L10" s="35"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="H12" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="41"/>
+      <c r="J14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="23">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1">
+        <v>65</v>
+      </c>
+      <c r="F15" s="21">
+        <f>E15/60</f>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="H15" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="43"/>
+      <c r="J15" s="25">
+        <v>30</v>
+      </c>
+      <c r="K15" s="1">
+        <v>230</v>
+      </c>
+      <c r="L15" s="26">
+        <f>K15/60</f>
+        <v>3.8333333333333335</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="23">
+        <v>20</v>
+      </c>
+      <c r="E16" s="1">
+        <v>400</v>
+      </c>
+      <c r="F16" s="22">
+        <f>E16/60</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="H16" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="43"/>
+      <c r="J16" s="25">
+        <v>20</v>
+      </c>
+      <c r="K16" s="1">
+        <v>493</v>
+      </c>
+      <c r="L16" s="27">
+        <f>K16/60</f>
+        <v>8.2166666666666668</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45">
+        <f>D15*F15+D16*F16</f>
+        <v>165.83333333333334</v>
+      </c>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="H18" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="46"/>
+      <c r="J18" s="35">
+        <f>J15*L15+J16*L16</f>
+        <v>279.33333333333337</v>
+      </c>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="24">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5608,18 +5758,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5632,6 +5770,18 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5699,12 +5849,12 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
       <c r="I4" s="51" t="s">
         <v>7</v>
       </c>
@@ -5765,20 +5915,20 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="4">
         <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="48"/>
+      <c r="J7" s="50"/>
       <c r="K7" s="4">
         <v>30</v>
       </c>
@@ -5787,20 +5937,20 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="48"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="4">
         <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="48"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="4">
         <v>20</v>
       </c>
@@ -5813,28 +5963,28 @@
         <v>5</v>
       </c>
       <c r="C10" s="44"/>
-      <c r="D10" s="49">
+      <c r="D10" s="47">
         <f>D7*E7 + D8*E8</f>
         <v>37.4</v>
       </c>
-      <c r="E10" s="49"/>
+      <c r="E10" s="47"/>
       <c r="I10" s="46" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="46"/>
-      <c r="K10" s="47">
+      <c r="K10" s="48">
         <f>K7*L7+K8*L8</f>
         <v>71.400000000000006</v>
       </c>
       <c r="L10" s="46"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
       <c r="I13" s="51" t="s">
         <v>19</v>
       </c>
@@ -5865,20 +6015,20 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="48"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="4">
         <v>30</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="48"/>
+      <c r="J16" s="50"/>
       <c r="K16" s="4">
         <v>30</v>
       </c>
@@ -5887,20 +6037,20 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="48"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="4">
         <v>20</v>
       </c>
       <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="I17" s="48" t="s">
+      <c r="I17" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="48"/>
+      <c r="J17" s="50"/>
       <c r="K17" s="4">
         <v>20</v>
       </c>
@@ -5913,16 +6063,16 @@
         <v>5</v>
       </c>
       <c r="C19" s="44"/>
-      <c r="D19" s="49">
+      <c r="D19" s="47">
         <f>D16*E16 + D17*E17</f>
         <v>120</v>
       </c>
-      <c r="E19" s="49"/>
+      <c r="E19" s="47"/>
       <c r="I19" s="46" t="s">
         <v>5</v>
       </c>
       <c r="J19" s="46"/>
-      <c r="K19" s="47">
+      <c r="K19" s="48">
         <f>K16*L16+K17*L17</f>
         <v>220</v>
       </c>
@@ -5942,6 +6092,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="I10:J10"/>
@@ -5954,18 +6116,6 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated personal docs jimmy
</commit_message>
<xml_diff>
--- a/reports/Tiempo estimado-real.xlsx
+++ b/reports/Tiempo estimado-real.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DP2\Documents\Workspace-24\Projects\Acme-SF-D02\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F55507-C170-41C1-B24B-E9615F4D6889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE97145B-B40E-4417-9FF9-C30FE5A00B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="4" r:id="rId1"/>
@@ -215,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -436,12 +436,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -529,17 +538,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -598,6 +607,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1964,7 +1975,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.7913834793950185E-2"/>
+          <c:y val="0.11974424075123323"/>
+          <c:w val="0.90231680899241073"/>
+          <c:h val="0.64548463887046492"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -2029,6 +2050,9 @@
                 <c:pt idx="1">
                   <c:v>110</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>360</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2099,6 +2123,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>388</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4667,16 +4694,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>730248</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>184522</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>110066</xdr:rowOff>
+      <xdr:rowOff>96058</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>687915</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>142189</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>31749</xdr:rowOff>
+      <xdr:rowOff>17741</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5005,7 +5032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D12626D-61D9-4105-9316-5A3F0038A1E8}">
   <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
@@ -5608,18 +5635,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5632,6 +5647,18 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5699,12 +5726,12 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
       <c r="I4" s="51" t="s">
         <v>7</v>
       </c>
@@ -5765,20 +5792,20 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="4">
         <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="48"/>
+      <c r="J7" s="50"/>
       <c r="K7" s="4">
         <v>30</v>
       </c>
@@ -5787,20 +5814,20 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="48"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="4">
         <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="48"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="4">
         <v>20</v>
       </c>
@@ -5813,28 +5840,28 @@
         <v>5</v>
       </c>
       <c r="C10" s="44"/>
-      <c r="D10" s="49">
+      <c r="D10" s="47">
         <f>D7*E7 + D8*E8</f>
         <v>37.4</v>
       </c>
-      <c r="E10" s="49"/>
+      <c r="E10" s="47"/>
       <c r="I10" s="46" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="46"/>
-      <c r="K10" s="47">
+      <c r="K10" s="48">
         <f>K7*L7+K8*L8</f>
         <v>71.400000000000006</v>
       </c>
       <c r="L10" s="46"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
       <c r="I13" s="51" t="s">
         <v>19</v>
       </c>
@@ -5865,20 +5892,20 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="48"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="4">
         <v>30</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="48"/>
+      <c r="J16" s="50"/>
       <c r="K16" s="4">
         <v>30</v>
       </c>
@@ -5887,20 +5914,20 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="48"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="4">
         <v>20</v>
       </c>
       <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="I17" s="48" t="s">
+      <c r="I17" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="48"/>
+      <c r="J17" s="50"/>
       <c r="K17" s="4">
         <v>20</v>
       </c>
@@ -5913,16 +5940,16 @@
         <v>5</v>
       </c>
       <c r="C19" s="44"/>
-      <c r="D19" s="49">
+      <c r="D19" s="47">
         <f>D16*E16 + D17*E17</f>
         <v>120</v>
       </c>
-      <c r="E19" s="49"/>
+      <c r="E19" s="47"/>
       <c r="I19" s="46" t="s">
         <v>5</v>
       </c>
       <c r="J19" s="46"/>
-      <c r="K19" s="47">
+      <c r="K19" s="48">
         <f>K16*L16+K17*L17</f>
         <v>220</v>
       </c>
@@ -5942,6 +5969,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="I10:J10"/>
@@ -5954,18 +5993,6 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6004,8 +6031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1538CD56-0247-4FF3-B2B1-3BAFD0549E9D}">
   <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6060,11 +6087,13 @@
       <c r="P4" s="13">
         <v>0</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="Q4" s="70">
+        <v>110</v>
+      </c>
+      <c r="R4" s="11">
         <f>E7+E8</f>
-        <v>110</v>
-      </c>
-      <c r="R4" s="11"/>
+        <v>360</v>
+      </c>
       <c r="S4" s="11"/>
       <c r="T4" s="12"/>
     </row>
@@ -6079,11 +6108,13 @@
       <c r="P5" s="14">
         <v>0</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="71">
+        <v>120</v>
+      </c>
+      <c r="R5" s="9">
         <f>K7+K8</f>
-        <v>120</v>
-      </c>
-      <c r="R5" s="9"/>
+        <v>388</v>
+      </c>
       <c r="S5" s="9"/>
       <c r="T5" s="10"/>
     </row>
@@ -6124,11 +6155,11 @@
         <v>30</v>
       </c>
       <c r="E7" s="1">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="F7" s="31">
         <f>E7/60</f>
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="H7" s="67" t="s">
         <v>2</v>
@@ -6138,11 +6169,11 @@
         <v>30</v>
       </c>
       <c r="K7" s="1">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="L7" s="34">
         <f>K7/60</f>
-        <v>1.1666666666666667</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -6154,12 +6185,11 @@
         <v>20</v>
       </c>
       <c r="E8" s="1">
-        <f>45+20</f>
-        <v>65</v>
+        <v>240</v>
       </c>
       <c r="F8" s="32">
         <f>E8/60</f>
-        <v>1.0833333333333333</v>
+        <v>4</v>
       </c>
       <c r="H8" s="67" t="s">
         <v>3</v>
@@ -6169,11 +6199,11 @@
         <v>20</v>
       </c>
       <c r="K8" s="1">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="L8" s="34">
         <f>K8/60</f>
-        <v>0.83333333333333337</v>
+        <v>4.166666666666667</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -6189,7 +6219,7 @@
       <c r="C10" s="59"/>
       <c r="D10" s="64">
         <f>D7*F7+D8*F8</f>
-        <v>44.166666666666664</v>
+        <v>140</v>
       </c>
       <c r="E10" s="64"/>
       <c r="F10" s="65"/>
@@ -6199,7 +6229,7 @@
       <c r="I10" s="69"/>
       <c r="J10" s="52">
         <f>J7*L7+J8*L8</f>
-        <v>51.666666666666671</v>
+        <v>152.33333333333334</v>
       </c>
       <c r="K10" s="52"/>
       <c r="L10" s="53"/>
@@ -6239,31 +6269,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
-      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{0376B26D-8886-44A8-809A-C3E816F8A869}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Hoja de Jimmy'!Q4:Q4</xm:f>
-              <xm:sqref>R4</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Hoja de Jimmy'!Q5:Q5</xm:f>
-              <xm:sqref>R5</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-      </x14:sparklineGroups>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: acabado dashboard administrador
</commit_message>
<xml_diff>
--- a/reports/Tiempo estimado-real.xlsx
+++ b/reports/Tiempo estimado-real.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace-24\Projects\Acme-SF-D01\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8654644A-F508-4CB1-9E5C-F261C1C22046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F05BFC-74C1-42B0-A112-ADB34407747B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
   </bookViews>
@@ -510,22 +510,11 @@
     <xf numFmtId="2" fontId="0" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -546,17 +535,32 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -615,10 +619,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1635,7 +1635,7 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1260</c:v>
+                  <c:v>1380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1712,7 +1712,7 @@
                   <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2460</c:v>
+                  <c:v>2670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5090,20 +5090,20 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="H4" s="45" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="H4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="43"/>
       <c r="O4" s="19" t="s">
         <v>8</v>
       </c>
@@ -5140,10 +5140,10 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -5153,10 +5153,10 @@
       <c r="F6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="48"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -5168,10 +5168,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -5182,10 +5182,10 @@
         <f>E7/60</f>
         <v>4.583333333333333</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="39"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -5198,10 +5198,10 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -5212,10 +5212,10 @@
         <f>E8/60</f>
         <v>3</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="39"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -5228,48 +5228,48 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41">
+      <c r="C10" s="48"/>
+      <c r="D10" s="49">
         <f>D7*F7+D8*F8</f>
         <v>197.5</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="H10" s="42" t="s">
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="H10" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="37">
+      <c r="I10" s="50"/>
+      <c r="J10" s="39">
         <f>J7*L7+J8*L8</f>
         <v>323.16666666666669</v>
       </c>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="H13" s="45" t="s">
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="H13" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="46"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="43"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="6" t="s">
         <v>17</v>
       </c>
@@ -5279,10 +5279,10 @@
       <c r="F15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I15" s="48"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="5" t="s">
         <v>17</v>
       </c>
@@ -5294,10 +5294,10 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="23">
         <v>30</v>
       </c>
@@ -5308,10 +5308,10 @@
         <f>E16/60</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="39"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="25">
         <v>30</v>
       </c>
@@ -5324,10 +5324,10 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="38"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="23">
         <v>20</v>
       </c>
@@ -5338,10 +5338,10 @@
         <f>E17/60</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="39"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="25">
         <v>20</v>
       </c>
@@ -5354,26 +5354,26 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41">
+      <c r="C19" s="48"/>
+      <c r="D19" s="49">
         <f>D16*F16+D17*F17</f>
         <v>165.83333333333334</v>
       </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="H19" s="42" t="s">
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="H19" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="37">
+      <c r="I19" s="50"/>
+      <c r="J19" s="39">
         <f>J16*L16+J17*L17</f>
         <v>279.33333333333337</v>
       </c>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -5389,6 +5389,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5401,18 +5413,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="H19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5467,30 +5467,30 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="H4" s="45" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="H4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="43"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -5500,10 +5500,10 @@
       <c r="F6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="48"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -5530,10 +5530,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -5544,10 +5544,10 @@
         <f>E7/60</f>
         <v>3.5</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="39"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -5576,10 +5576,10 @@
       <c r="T7" s="12"/>
     </row>
     <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -5591,10 +5591,10 @@
         <f>E8/60</f>
         <v>3</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="39"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -5623,46 +5623,46 @@
       <c r="T8" s="10"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41">
+      <c r="C10" s="48"/>
+      <c r="D10" s="49">
         <f>D7*F7+D8*F8</f>
         <v>165</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="H10" s="42" t="s">
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="H10" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="37">
+      <c r="I10" s="50"/>
+      <c r="J10" s="39">
         <f>J7*L7+J8*L8</f>
         <v>205.33333333333334</v>
       </c>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="H12" s="45" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="H12" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="46"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="43"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
@@ -5671,10 +5671,10 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="47"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
@@ -5684,10 +5684,10 @@
       <c r="F14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="48" t="s">
+      <c r="H14" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="48"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
@@ -5699,10 +5699,10 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="38"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="23">
         <v>30</v>
       </c>
@@ -5713,10 +5713,10 @@
         <f>E15/60</f>
         <v>3.5</v>
       </c>
-      <c r="H15" s="39" t="s">
+      <c r="H15" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="39"/>
+      <c r="I15" s="47"/>
       <c r="J15" s="25">
         <v>30</v>
       </c>
@@ -5729,10 +5729,10 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="23">
         <v>20</v>
       </c>
@@ -5744,10 +5744,10 @@
         <f>E16/60</f>
         <v>15.166666666666666</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="39"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="25">
         <v>20</v>
       </c>
@@ -5760,26 +5760,26 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41">
+      <c r="C18" s="48"/>
+      <c r="D18" s="49">
         <f>D15*F15+D16*F16</f>
         <v>408.33333333333331</v>
       </c>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="H18" s="42" t="s">
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="H18" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="42"/>
-      <c r="J18" s="37">
+      <c r="I18" s="50"/>
+      <c r="J18" s="39">
         <f>J15*L15+J16*L16</f>
         <v>368.83333333333331</v>
       </c>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -5795,6 +5795,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5807,18 +5819,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5856,7 +5856,7 @@
   <dimension ref="B2:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5886,18 +5886,18 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="I4" s="53" t="s">
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="I4" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
       <c r="O4" s="7" t="s">
         <v>8</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>300</v>
       </c>
       <c r="S4" s="11">
-        <v>1260</v>
+        <v>1380</v>
       </c>
       <c r="T4" s="12"/>
     </row>
@@ -5929,25 +5929,25 @@
         <v>540</v>
       </c>
       <c r="S5" s="9">
-        <v>2460</v>
+        <v>2670</v>
       </c>
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="48"/>
+      <c r="J6" s="45"/>
       <c r="K6" s="5" t="s">
         <v>1</v>
       </c>
@@ -6000,54 +6000,54 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="49">
+      <c r="C10" s="48"/>
+      <c r="D10" s="53">
         <f>D7*E7 + D8*E8</f>
         <v>37.4</v>
       </c>
-      <c r="E10" s="49"/>
-      <c r="I10" s="42" t="s">
+      <c r="E10" s="53"/>
+      <c r="I10" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="42"/>
-      <c r="K10" s="50">
+      <c r="J10" s="50"/>
+      <c r="K10" s="51">
         <f>K7*L7+K8*L8</f>
         <v>71.400000000000006</v>
       </c>
-      <c r="L10" s="42"/>
+      <c r="L10" s="50"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="I13" s="53" t="s">
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="I13" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="48"/>
+      <c r="J15" s="45"/>
       <c r="K15" s="5" t="s">
         <v>1</v>
       </c>
@@ -6100,24 +6100,24 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="49">
+      <c r="C19" s="48"/>
+      <c r="D19" s="53">
         <f>D16*E16 + D17*E17</f>
         <v>120</v>
       </c>
-      <c r="E19" s="49"/>
-      <c r="I19" s="42" t="s">
+      <c r="E19" s="53"/>
+      <c r="I19" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="42"/>
-      <c r="K19" s="50">
+      <c r="J19" s="50"/>
+      <c r="K19" s="51">
         <f>K16*L16+K17*L17</f>
         <v>220</v>
       </c>
-      <c r="L19" s="42"/>
+      <c r="L19" s="50"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -6132,34 +6132,34 @@
       <c r="E21" s="3"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="I23" s="53" t="s">
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="I23" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="47"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="48" t="s">
+      <c r="I25" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="J25" s="48"/>
+      <c r="J25" s="45"/>
       <c r="K25" s="5" t="s">
         <v>1</v>
       </c>
@@ -6175,7 +6175,7 @@
       <c r="D26" s="4">
         <v>30</v>
       </c>
-      <c r="E26" s="72">
+      <c r="E26" s="37">
         <v>4</v>
       </c>
       <c r="I26" s="52" t="s">
@@ -6185,7 +6185,7 @@
       <c r="K26" s="4">
         <v>30</v>
       </c>
-      <c r="L26" s="72">
+      <c r="L26" s="37">
         <v>6</v>
       </c>
     </row>
@@ -6197,8 +6197,8 @@
       <c r="D27" s="4">
         <v>20</v>
       </c>
-      <c r="E27" s="72">
-        <v>17</v>
+      <c r="E27" s="37">
+        <v>19</v>
       </c>
       <c r="I27" s="52" t="s">
         <v>3</v>
@@ -6207,59 +6207,35 @@
       <c r="K27" s="4">
         <v>20</v>
       </c>
-      <c r="L27" s="72">
-        <v>35</v>
+      <c r="L27" s="37">
+        <v>38.5</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L28" s="73"/>
+      <c r="L28" s="38"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="49">
+      <c r="C29" s="48"/>
+      <c r="D29" s="53">
         <f>D26*E26 + D27*E27</f>
-        <v>460</v>
-      </c>
-      <c r="E29" s="49"/>
-      <c r="I29" s="42" t="s">
+        <v>500</v>
+      </c>
+      <c r="E29" s="53"/>
+      <c r="I29" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="42"/>
-      <c r="K29" s="50">
+      <c r="J29" s="50"/>
+      <c r="K29" s="51">
         <f>K26*L26+K27*L27</f>
-        <v>880</v>
-      </c>
-      <c r="L29" s="42"/>
+        <v>950</v>
+      </c>
+      <c r="L29" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="I16:J16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="I10:J10"/>
@@ -6272,6 +6248,30 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="I29:J29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6346,20 +6346,20 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65"/>
-      <c r="H4" s="56" t="s">
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="67"/>
+      <c r="H4" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="58"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="60"/>
       <c r="O4" s="19" t="s">
         <v>8</v>
       </c>
@@ -6398,10 +6398,10 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -6411,10 +6411,10 @@
       <c r="F6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="48"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -6426,10 +6426,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -6440,10 +6440,10 @@
         <f>E7/60</f>
         <v>2</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="39"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -6456,10 +6456,10 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -6470,10 +6470,10 @@
         <f>E8/60</f>
         <v>4</v>
       </c>
-      <c r="H8" s="69" t="s">
+      <c r="H8" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="39"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -6492,26 +6492,26 @@
       <c r="L9" s="29"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="66">
+      <c r="C10" s="63"/>
+      <c r="D10" s="68">
         <f>D7*F7+D8*F8</f>
         <v>140</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="67"/>
-      <c r="H10" s="70" t="s">
+      <c r="E10" s="68"/>
+      <c r="F10" s="69"/>
+      <c r="H10" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="71"/>
-      <c r="J10" s="54">
+      <c r="I10" s="73"/>
+      <c r="J10" s="56">
         <f>J7*L7+J8*L8</f>
         <v>152.33333333333334</v>
       </c>
-      <c r="K10" s="54"/>
-      <c r="L10" s="55"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="57"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>

</xml_diff>

<commit_message>
feat: Ultimo cambio en el csv
</commit_message>
<xml_diff>
--- a/reports/Tiempo estimado-real.xlsx
+++ b/reports/Tiempo estimado-real.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DP2\Documents\Workspace-24\Projects\Acme-SF-D03\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace-24\Projects\Acme-SF-D04\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C989D8B-4404-4AFC-B74A-FF396A346BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96323016-E243-4BFD-9810-DEED8054B385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="26">
   <si>
     <t>Rol</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Tiempo estimado D3</t>
+  </si>
+  <si>
+    <t>Tiempo estimado D04</t>
+  </si>
+  <si>
+    <t>Tiempo real D04</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -527,41 +552,29 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,7 +585,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -581,28 +597,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -611,10 +609,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1639,6 +1645,9 @@
                 <c:pt idx="3">
                   <c:v>1380</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>1260</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1715,6 +1724,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2670</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5098,20 +5110,20 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="H4" s="40" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="H4" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="41"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="48"/>
       <c r="O4" s="19" t="s">
         <v>8</v>
       </c>
@@ -5148,10 +5160,10 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -5161,10 +5173,10 @@
       <c r="F6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="43"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -5176,10 +5188,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -5190,10 +5202,10 @@
         <f>E7/60</f>
         <v>4.583333333333333</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="45"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -5206,10 +5218,10 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -5220,10 +5232,10 @@
         <f>E8/60</f>
         <v>3</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="45"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -5236,48 +5248,48 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47">
+      <c r="C10" s="42"/>
+      <c r="D10" s="43">
         <f>D7*F7+D8*F8</f>
         <v>197.5</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="H10" s="48" t="s">
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="H10" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="37">
+      <c r="I10" s="44"/>
+      <c r="J10" s="39">
         <f>J7*L7+J8*L8</f>
         <v>323.16666666666669</v>
       </c>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="H13" s="40" t="s">
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="H13" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="41"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="42"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="6" t="s">
         <v>17</v>
       </c>
@@ -5287,10 +5299,10 @@
       <c r="F15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="I15" s="43"/>
+      <c r="I15" s="50"/>
       <c r="J15" s="5" t="s">
         <v>17</v>
       </c>
@@ -5302,10 +5314,10 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="23">
         <v>30</v>
       </c>
@@ -5316,10 +5328,10 @@
         <f>E16/60</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="H16" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="45"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="25">
         <v>30</v>
       </c>
@@ -5332,10 +5344,10 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="44"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="23">
         <v>20</v>
       </c>
@@ -5346,10 +5358,10 @@
         <f>E17/60</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="H17" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="45"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="25">
         <v>20</v>
       </c>
@@ -5362,26 +5374,26 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47">
+      <c r="C19" s="42"/>
+      <c r="D19" s="43">
         <f>D16*F16+D17*F17</f>
         <v>165.83333333333334</v>
       </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="H19" s="48" t="s">
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="H19" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="37">
+      <c r="I19" s="44"/>
+      <c r="J19" s="39">
         <f>J16*L16+J17*L17</f>
         <v>279.33333333333337</v>
       </c>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -5397,18 +5409,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H16:I16"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5421,6 +5421,18 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="H19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5475,30 +5487,30 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="H4" s="40" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="H4" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="41"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="48"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -5508,10 +5520,10 @@
       <c r="F6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="43"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -5538,10 +5550,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -5552,10 +5564,10 @@
         <f>E7/60</f>
         <v>3.5</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="45"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -5587,10 +5599,10 @@
       <c r="T7" s="12"/>
     </row>
     <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -5602,10 +5614,10 @@
         <f>E8/60</f>
         <v>3</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="45"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -5637,46 +5649,46 @@
       <c r="T8" s="10"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47">
+      <c r="C10" s="42"/>
+      <c r="D10" s="43">
         <f>D7*F7+D8*F8</f>
         <v>165</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="H10" s="48" t="s">
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="H10" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="37">
+      <c r="I10" s="44"/>
+      <c r="J10" s="39">
         <f>J7*L7+J8*L8</f>
         <v>205.33333333333334</v>
       </c>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="H12" s="40" t="s">
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="H12" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="41"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="48"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
@@ -5685,10 +5697,10 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="42"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
@@ -5698,10 +5710,10 @@
       <c r="F14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="43"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
@@ -5713,10 +5725,10 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="44"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="23">
         <v>30</v>
       </c>
@@ -5727,10 +5739,10 @@
         <f>E15/60</f>
         <v>3.5</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="45"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="25">
         <v>30</v>
       </c>
@@ -5743,10 +5755,10 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="23">
         <v>20</v>
       </c>
@@ -5758,10 +5770,10 @@
         <f>E16/60</f>
         <v>15.166666666666666</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="H16" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="45"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="25">
         <v>20</v>
       </c>
@@ -5774,52 +5786,52 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="47">
+      <c r="C18" s="42"/>
+      <c r="D18" s="43">
         <f>D15*F15+D16*F16</f>
         <v>408.33333333333331</v>
       </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="H18" s="48" t="s">
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="H18" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="48"/>
-      <c r="J18" s="37">
+      <c r="I18" s="44"/>
+      <c r="J18" s="39">
         <f>J15*L15+J16*L16</f>
         <v>368.83333333333331</v>
       </c>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="H20" s="40" t="s">
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="H20" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="41"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="48"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="42"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="6" t="s">
         <v>17</v>
       </c>
@@ -5829,10 +5841,10 @@
       <c r="F22" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="43" t="s">
+      <c r="H22" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="43"/>
+      <c r="I22" s="50"/>
       <c r="J22" s="5" t="s">
         <v>17</v>
       </c>
@@ -5844,10 +5856,10 @@
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="44"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="23">
         <v>30</v>
       </c>
@@ -5858,10 +5870,10 @@
         <f>E23/60</f>
         <v>3.5</v>
       </c>
-      <c r="H23" s="45" t="s">
+      <c r="H23" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="I23" s="45"/>
+      <c r="I23" s="41"/>
       <c r="J23" s="25">
         <v>30</v>
       </c>
@@ -5874,10 +5886,10 @@
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="44"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="23">
         <v>20</v>
       </c>
@@ -5889,10 +5901,10 @@
         <f>E24/60</f>
         <v>15.166666666666666</v>
       </c>
-      <c r="H24" s="45" t="s">
+      <c r="H24" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="45"/>
+      <c r="I24" s="41"/>
       <c r="J24" s="25">
         <v>20</v>
       </c>
@@ -5905,41 +5917,41 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="47">
+      <c r="C26" s="42"/>
+      <c r="D26" s="43">
         <f>D23*F23+D24*F24</f>
         <v>408.33333333333331</v>
       </c>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="H26" s="48" t="s">
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="H26" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="48"/>
-      <c r="J26" s="37">
+      <c r="I26" s="44"/>
+      <c r="J26" s="39">
         <f>J23*L23+J24*L24</f>
         <v>526.83333333333326</v>
       </c>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H23:I23"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5952,18 +5964,18 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5998,10 +6010,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12886396-CDAF-4037-9656-80B26E0CDA1B}">
-  <dimension ref="B2:T29"/>
+  <dimension ref="B2:T38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6031,18 +6043,18 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="I4" s="53" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="I4" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
       <c r="O4" s="7" t="s">
         <v>8</v>
       </c>
@@ -6058,7 +6070,9 @@
       <c r="S4" s="11">
         <v>1380</v>
       </c>
-      <c r="T4" s="12"/>
+      <c r="T4" s="12">
+        <v>1260</v>
+      </c>
     </row>
     <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O5" s="8" t="s">
@@ -6076,23 +6090,25 @@
       <c r="S5" s="9">
         <v>2670</v>
       </c>
-      <c r="T5" s="10"/>
+      <c r="T5" s="10">
+        <v>1800</v>
+      </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="43"/>
+      <c r="J6" s="50"/>
       <c r="K6" s="5" t="s">
         <v>1</v>
       </c>
@@ -6101,20 +6117,20 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="50"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="4">
         <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="50"/>
+      <c r="J7" s="54"/>
       <c r="K7" s="4">
         <v>30</v>
       </c>
@@ -6123,20 +6139,20 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="50"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="4">
         <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="50"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="4">
         <v>20</v>
       </c>
@@ -6145,54 +6161,54 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="51">
         <f>D7*E7 + D8*E8</f>
         <v>37.4</v>
       </c>
       <c r="E10" s="51"/>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="48"/>
-      <c r="K10" s="49">
+      <c r="J10" s="44"/>
+      <c r="K10" s="52">
         <f>K7*L7+K8*L8</f>
         <v>71.400000000000006</v>
       </c>
-      <c r="L10" s="48"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="I13" s="53" t="s">
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="I13" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="42"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="43"/>
+      <c r="J15" s="50"/>
       <c r="K15" s="5" t="s">
         <v>1</v>
       </c>
@@ -6201,20 +6217,20 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="50"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="4">
         <v>30</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="I16" s="50" t="s">
+      <c r="I16" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="50"/>
+      <c r="J16" s="54"/>
       <c r="K16" s="4">
         <v>30</v>
       </c>
@@ -6223,20 +6239,20 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="4">
         <v>20</v>
       </c>
       <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="I17" s="50" t="s">
+      <c r="I17" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="50"/>
+      <c r="J17" s="54"/>
       <c r="K17" s="4">
         <v>20</v>
       </c>
@@ -6245,24 +6261,24 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="46"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="51">
         <f>D16*E16 + D17*E17</f>
         <v>120</v>
       </c>
       <c r="E19" s="51"/>
-      <c r="I19" s="48" t="s">
+      <c r="I19" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="48"/>
-      <c r="K19" s="49">
+      <c r="J19" s="44"/>
+      <c r="K19" s="52">
         <f>K16*L16+K17*L17</f>
         <v>220</v>
       </c>
-      <c r="L19" s="48"/>
+      <c r="L19" s="44"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -6277,34 +6293,34 @@
       <c r="E21" s="3"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="I23" s="53" t="s">
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="I23" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="42"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="43" t="s">
+      <c r="I25" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="J25" s="43"/>
+      <c r="J25" s="50"/>
       <c r="K25" s="5" t="s">
         <v>1</v>
       </c>
@@ -6313,20 +6329,20 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="50"/>
+      <c r="C26" s="54"/>
       <c r="D26" s="4">
         <v>30</v>
       </c>
       <c r="E26" s="35">
         <v>4</v>
       </c>
-      <c r="I26" s="50" t="s">
+      <c r="I26" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="J26" s="50"/>
+      <c r="J26" s="54"/>
       <c r="K26" s="4">
         <v>30</v>
       </c>
@@ -6335,20 +6351,20 @@
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="50"/>
+      <c r="C27" s="54"/>
       <c r="D27" s="4">
         <v>20</v>
       </c>
       <c r="E27" s="35">
         <v>19</v>
       </c>
-      <c r="I27" s="50" t="s">
+      <c r="I27" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="J27" s="50"/>
+      <c r="J27" s="54"/>
       <c r="K27" s="4">
         <v>20</v>
       </c>
@@ -6360,27 +6376,166 @@
       <c r="L28" s="36"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="46"/>
+      <c r="C29" s="42"/>
       <c r="D29" s="51">
         <f>D26*E26 + D27*E27</f>
         <v>500</v>
       </c>
       <c r="E29" s="51"/>
-      <c r="I29" s="48" t="s">
+      <c r="I29" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="48"/>
-      <c r="K29" s="49">
+      <c r="J29" s="44"/>
+      <c r="K29" s="52">
         <f>K26*L26+K27*L27</f>
         <v>950</v>
       </c>
-      <c r="L29" s="48"/>
+      <c r="L29" s="44"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="I32" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="55"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="49"/>
+      <c r="D34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" s="50"/>
+      <c r="K34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="54"/>
+      <c r="D35" s="4">
+        <v>30</v>
+      </c>
+      <c r="E35" s="35">
+        <v>6</v>
+      </c>
+      <c r="I35" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" s="54"/>
+      <c r="K35" s="4">
+        <v>30</v>
+      </c>
+      <c r="L35" s="35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="54"/>
+      <c r="D36" s="4">
+        <v>20</v>
+      </c>
+      <c r="E36" s="35">
+        <v>15</v>
+      </c>
+      <c r="I36" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" s="54"/>
+      <c r="K36" s="4">
+        <v>20</v>
+      </c>
+      <c r="L36" s="35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L37" s="36"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="42"/>
+      <c r="D38" s="51">
+        <f>D35*E35 + D36*E36</f>
+        <v>480</v>
+      </c>
+      <c r="E38" s="51"/>
+      <c r="I38" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" s="44"/>
+      <c r="K38" s="52">
+        <f>K35*L35+K36*L36</f>
+        <v>660</v>
+      </c>
+      <c r="L38" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="48">
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="I32:L32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="I10:J10"/>
@@ -6393,30 +6548,6 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="I29:J29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6455,7 +6586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1538CD56-0247-4FF3-B2B1-3BAFD0549E9D}">
   <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
@@ -6491,20 +6622,20 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65"/>
-      <c r="H4" s="56" t="s">
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="58"/>
+      <c r="H4" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="58"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="61"/>
       <c r="O4" s="19" t="s">
         <v>8</v>
       </c>
@@ -6542,7 +6673,7 @@
         <f>K7+K8</f>
         <v>388</v>
       </c>
-      <c r="S5" s="73">
+      <c r="S5" s="38">
         <f>K15+K16</f>
         <v>1699</v>
       </c>
@@ -6552,7 +6683,7 @@
       <c r="B6" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -6562,10 +6693,10 @@
       <c r="F6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="43"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -6577,10 +6708,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -6591,10 +6722,10 @@
         <f>E7/60</f>
         <v>2</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="45"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -6607,10 +6738,10 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -6621,10 +6752,10 @@
         <f>E8/60</f>
         <v>4</v>
       </c>
-      <c r="H8" s="69" t="s">
+      <c r="H8" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="45"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -6643,43 +6774,43 @@
       <c r="L9" s="29"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="61"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="66">
         <f>D7*F7+D8*F8</f>
         <v>140</v>
       </c>
       <c r="E10" s="66"/>
       <c r="F10" s="67"/>
-      <c r="H10" s="70" t="s">
+      <c r="H10" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="71"/>
-      <c r="J10" s="54">
+      <c r="I10" s="69"/>
+      <c r="J10" s="70">
         <f>J7*L7+J8*L8</f>
         <v>152.33333333333334</v>
       </c>
-      <c r="K10" s="54"/>
-      <c r="L10" s="55"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="71"/>
     </row>
     <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
-      <c r="H12" s="56" t="s">
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+      <c r="H12" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="58"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="61"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
@@ -6691,7 +6822,7 @@
       <c r="B14" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="42"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
@@ -6701,10 +6832,10 @@
       <c r="F14" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="68" t="s">
+      <c r="H14" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="43"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
@@ -6716,10 +6847,10 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="44"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="23">
         <v>30</v>
       </c>
@@ -6730,10 +6861,10 @@
         <f>E15/60</f>
         <v>4</v>
       </c>
-      <c r="H15" s="69" t="s">
+      <c r="H15" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="45"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="25">
         <v>30</v>
       </c>
@@ -6746,10 +6877,10 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="23">
         <v>20</v>
       </c>
@@ -6760,14 +6891,14 @@
         <f>E16/60</f>
         <v>16</v>
       </c>
-      <c r="H16" s="69" t="s">
+      <c r="H16" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="45"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="25">
         <v>20</v>
       </c>
-      <c r="K16" s="72">
+      <c r="K16" s="37">
         <v>1442</v>
       </c>
       <c r="L16" s="34">
@@ -6782,26 +6913,26 @@
       <c r="L17" s="29"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="65"/>
       <c r="D18" s="66">
         <f>D15*F15+D16*F16</f>
         <v>440</v>
       </c>
       <c r="E18" s="66"/>
       <c r="F18" s="67"/>
-      <c r="H18" s="70" t="s">
+      <c r="H18" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="71"/>
-      <c r="J18" s="54">
+      <c r="I18" s="69"/>
+      <c r="J18" s="70">
         <f>J15*L15+J16*L16</f>
         <v>609.16666666666674</v>
       </c>
-      <c r="K18" s="54"/>
-      <c r="L18" s="55"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="71"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -6823,6 +6954,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="H12:L12"/>
     <mergeCell ref="B14:C14"/>
@@ -6835,18 +6978,6 @@
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
- Finalizacion de entrega Student 1
Signed-off-by: IsmaelGata <isgatdor@alum.us.es>
</commit_message>
<xml_diff>
--- a/reports/Tiempo estimado-real.xlsx
+++ b/reports/Tiempo estimado-real.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace-24\Projects\Acme-SF-D04\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismae\Documents\Universidad de Sevilla\DISEÑO Y PRUEBAS II\Workspace-24\Projects\Acme-SF-D04\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D773AF6A-948B-4537-B22E-7ADEC6DE7F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9137E4-8F12-4A72-A151-1C2E06CB3C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{08F9934D-43B2-436E-8607-F2E43C784395}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="27">
   <si>
     <t>Rol</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Tiempo real D04</t>
+  </si>
+  <si>
+    <t>Tiempo estimado D4</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -516,22 +519,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -552,20 +558,62 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,49 +624,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1214,6 +1235,9 @@
                 <c:pt idx="3">
                   <c:v>1120</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>930</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1290,6 +1314,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5110,20 +5137,20 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="H4" s="47" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="H4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="49"/>
       <c r="O4" s="19" t="s">
         <v>8</v>
       </c>
@@ -5160,10 +5187,10 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -5173,10 +5200,10 @@
       <c r="F6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -5188,10 +5215,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="40"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -5202,10 +5229,10 @@
         <f>E7/60</f>
         <v>4.583333333333333</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="41"/>
+      <c r="I7" s="53"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -5218,10 +5245,10 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -5232,10 +5259,10 @@
         <f>E8/60</f>
         <v>3</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="41"/>
+      <c r="I8" s="53"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -5248,48 +5275,48 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="43">
+      <c r="C10" s="54"/>
+      <c r="D10" s="55">
         <f>D7*F7+D8*F8</f>
         <v>197.5</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="H10" s="44" t="s">
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="H10" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="44"/>
-      <c r="J10" s="39">
+      <c r="I10" s="56"/>
+      <c r="J10" s="45">
         <f>J7*L7+J8*L8</f>
         <v>323.16666666666669</v>
       </c>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="H13" s="47" t="s">
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="H13" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="49"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="6" t="s">
         <v>17</v>
       </c>
@@ -5299,10 +5326,10 @@
       <c r="F15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="50" t="s">
+      <c r="H15" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="I15" s="50"/>
+      <c r="I15" s="51"/>
       <c r="J15" s="5" t="s">
         <v>17</v>
       </c>
@@ -5314,10 +5341,10 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="23">
         <v>30</v>
       </c>
@@ -5328,10 +5355,10 @@
         <f>E16/60</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="41"/>
+      <c r="I16" s="53"/>
       <c r="J16" s="25">
         <v>30</v>
       </c>
@@ -5344,10 +5371,10 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="40"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="23">
         <v>20</v>
       </c>
@@ -5358,10 +5385,10 @@
         <f>E17/60</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="H17" s="41" t="s">
+      <c r="H17" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="41"/>
+      <c r="I17" s="53"/>
       <c r="J17" s="25">
         <v>20</v>
       </c>
@@ -5374,26 +5401,26 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43">
+      <c r="C19" s="54"/>
+      <c r="D19" s="55">
         <f>D16*F16+D17*F17</f>
         <v>165.83333333333334</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="H19" s="44" t="s">
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="H19" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="39">
+      <c r="I19" s="56"/>
+      <c r="J19" s="45">
         <f>J16*L16+J17*L17</f>
         <v>279.33333333333337</v>
       </c>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -5409,6 +5436,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5421,18 +5460,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="H19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5467,10 +5494,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9AF520-1A94-4357-9CE4-04F00D982623}">
-  <dimension ref="B4:T26"/>
+  <dimension ref="B4:T34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5487,30 +5514,30 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="H4" s="47" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="H4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="49"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -5520,10 +5547,10 @@
       <c r="F6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -5550,10 +5577,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="40"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -5564,10 +5591,10 @@
         <f>E7/60</f>
         <v>3.5</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="41"/>
+      <c r="I7" s="53"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -5596,13 +5623,16 @@
         <f>E23+E24</f>
         <v>1120</v>
       </c>
-      <c r="T7" s="12"/>
+      <c r="T7" s="12">
+        <f>E31+E32</f>
+        <v>930</v>
+      </c>
     </row>
     <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -5614,10 +5644,10 @@
         <f>E8/60</f>
         <v>3</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="41"/>
+      <c r="I8" s="53"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -5646,49 +5676,52 @@
         <f>K23+K24</f>
         <v>1500</v>
       </c>
-      <c r="T8" s="10"/>
+      <c r="T8" s="10">
+        <f>K31+K32</f>
+        <v>2370</v>
+      </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="43">
+      <c r="C10" s="54"/>
+      <c r="D10" s="55">
         <f>D7*F7+D8*F8</f>
         <v>165</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="H10" s="44" t="s">
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="H10" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="44"/>
-      <c r="J10" s="39">
+      <c r="I10" s="56"/>
+      <c r="J10" s="45">
         <f>J7*L7+J8*L8</f>
         <v>205.33333333333334</v>
       </c>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="H12" s="47" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="H12" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="49"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
@@ -5697,10 +5730,10 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
@@ -5710,10 +5743,10 @@
       <c r="F14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="50" t="s">
+      <c r="H14" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="50"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
@@ -5725,10 +5758,10 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="23">
         <v>30</v>
       </c>
@@ -5739,10 +5772,10 @@
         <f>E15/60</f>
         <v>3.5</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="41"/>
+      <c r="I15" s="53"/>
       <c r="J15" s="25">
         <v>30</v>
       </c>
@@ -5755,10 +5788,10 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="23">
         <v>20</v>
       </c>
@@ -5770,10 +5803,10 @@
         <f>E16/60</f>
         <v>15.166666666666666</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="41"/>
+      <c r="I16" s="53"/>
       <c r="J16" s="25">
         <v>20</v>
       </c>
@@ -5786,52 +5819,52 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43">
+      <c r="C18" s="54"/>
+      <c r="D18" s="55">
         <f>D15*F15+D16*F16</f>
         <v>408.33333333333331</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="H18" s="44" t="s">
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="H18" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="44"/>
-      <c r="J18" s="39">
+      <c r="I18" s="56"/>
+      <c r="J18" s="45">
         <f>J15*L15+J16*L16</f>
         <v>368.83333333333331</v>
       </c>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="H20" s="47" t="s">
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="H20" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="49"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="49"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="6" t="s">
         <v>17</v>
       </c>
@@ -5841,10 +5874,10 @@
       <c r="F22" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="50" t="s">
+      <c r="H22" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="50"/>
+      <c r="I22" s="51"/>
       <c r="J22" s="5" t="s">
         <v>17</v>
       </c>
@@ -5856,10 +5889,10 @@
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="40"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="23">
         <v>30</v>
       </c>
@@ -5870,10 +5903,10 @@
         <f>E23/60</f>
         <v>3.5</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="I23" s="41"/>
+      <c r="I23" s="53"/>
       <c r="J23" s="25">
         <v>30</v>
       </c>
@@ -5886,10 +5919,10 @@
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="40"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="23">
         <v>20</v>
       </c>
@@ -5901,10 +5934,10 @@
         <f>E24/60</f>
         <v>15.166666666666666</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="H24" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="41"/>
+      <c r="I24" s="53"/>
       <c r="J24" s="25">
         <v>20</v>
       </c>
@@ -5917,41 +5950,171 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43">
+      <c r="C26" s="54"/>
+      <c r="D26" s="55">
         <f>D23*F23+D24*F24</f>
         <v>408.33333333333331</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="H26" s="44" t="s">
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="H26" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="44"/>
-      <c r="J26" s="39">
+      <c r="I26" s="56"/>
+      <c r="J26" s="45">
         <f>J23*L23+J24*L24</f>
         <v>526.83333333333326</v>
       </c>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="H28" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="44"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="39"/>
+      <c r="D31" s="23">
+        <v>30</v>
+      </c>
+      <c r="E31" s="1">
+        <v>90</v>
+      </c>
+      <c r="F31" s="21">
+        <f>E31/60</f>
+        <v>1.5</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="40"/>
+      <c r="J31" s="25">
+        <v>30</v>
+      </c>
+      <c r="K31" s="1">
+        <v>117</v>
+      </c>
+      <c r="L31" s="26">
+        <f>K31/60</f>
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="39"/>
+      <c r="D32" s="23">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1">
+        <v>840</v>
+      </c>
+      <c r="F32" s="22">
+        <f>E32/60</f>
+        <v>14</v>
+      </c>
+      <c r="H32" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="40"/>
+      <c r="J32" s="25">
+        <v>20</v>
+      </c>
+      <c r="K32" s="1">
+        <v>2253</v>
+      </c>
+      <c r="L32" s="27">
+        <f>K32/60</f>
+        <v>37.549999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="54"/>
+      <c r="D34" s="55">
+        <f>D31*F31+D32*F32</f>
+        <v>325</v>
+      </c>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="H34" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" s="56"/>
+      <c r="J34" s="45">
+        <f>J31*L31+J32*L32</f>
+        <v>809.5</v>
+      </c>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H23:I23"/>
+  <mergeCells count="40">
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
@@ -5964,18 +6127,18 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="H26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6012,8 +6175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12886396-CDAF-4037-9656-80B26E0CDA1B}">
   <dimension ref="B2:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6043,18 +6206,18 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="I4" s="55" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="I4" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
       <c r="O4" s="7" t="s">
         <v>8</v>
       </c>
@@ -6095,20 +6258,20 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="I6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="50"/>
+      <c r="J6" s="51"/>
       <c r="K6" s="5" t="s">
         <v>1</v>
       </c>
@@ -6117,20 +6280,20 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="54"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="4">
         <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="54"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="4">
         <v>30</v>
       </c>
@@ -6139,20 +6302,20 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="54"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="4">
         <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="58"/>
       <c r="K8" s="4">
         <v>20</v>
       </c>
@@ -6161,54 +6324,54 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="51">
+      <c r="C10" s="54"/>
+      <c r="D10" s="59">
         <f>D7*E7 + D8*E8</f>
         <v>37.4</v>
       </c>
-      <c r="E10" s="51"/>
-      <c r="I10" s="44" t="s">
+      <c r="E10" s="59"/>
+      <c r="I10" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="44"/>
-      <c r="K10" s="52">
+      <c r="J10" s="56"/>
+      <c r="K10" s="57">
         <f>K7*L7+K8*L8</f>
         <v>71.400000000000006</v>
       </c>
-      <c r="L10" s="44"/>
+      <c r="L10" s="56"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="I13" s="55" t="s">
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="I13" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="50" t="s">
+      <c r="I15" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="50"/>
+      <c r="J15" s="51"/>
       <c r="K15" s="5" t="s">
         <v>1</v>
       </c>
@@ -6217,20 +6380,20 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="4">
         <v>30</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="54"/>
+      <c r="J16" s="58"/>
       <c r="K16" s="4">
         <v>30</v>
       </c>
@@ -6239,20 +6402,20 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="54"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="4">
         <v>20</v>
       </c>
       <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="I17" s="54" t="s">
+      <c r="I17" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="54"/>
+      <c r="J17" s="58"/>
       <c r="K17" s="4">
         <v>20</v>
       </c>
@@ -6261,24 +6424,24 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="51">
+      <c r="C19" s="54"/>
+      <c r="D19" s="59">
         <f>D16*E16 + D17*E17</f>
         <v>120</v>
       </c>
-      <c r="E19" s="51"/>
-      <c r="I19" s="44" t="s">
+      <c r="E19" s="59"/>
+      <c r="I19" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="44"/>
-      <c r="K19" s="52">
+      <c r="J19" s="56"/>
+      <c r="K19" s="57">
         <f>K16*L16+K17*L17</f>
         <v>220</v>
       </c>
-      <c r="L19" s="44"/>
+      <c r="L19" s="56"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -6293,34 +6456,34 @@
       <c r="E21" s="3"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="I23" s="55" t="s">
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="I23" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="50" t="s">
+      <c r="I25" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="J25" s="50"/>
+      <c r="J25" s="51"/>
       <c r="K25" s="5" t="s">
         <v>1</v>
       </c>
@@ -6329,20 +6492,20 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="54"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="4">
         <v>30</v>
       </c>
       <c r="E26" s="35">
         <v>4</v>
       </c>
-      <c r="I26" s="54" t="s">
+      <c r="I26" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="J26" s="54"/>
+      <c r="J26" s="58"/>
       <c r="K26" s="4">
         <v>30</v>
       </c>
@@ -6351,20 +6514,20 @@
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="54"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="4">
         <v>20</v>
       </c>
       <c r="E27" s="35">
         <v>19</v>
       </c>
-      <c r="I27" s="54" t="s">
+      <c r="I27" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J27" s="54"/>
+      <c r="J27" s="58"/>
       <c r="K27" s="4">
         <v>20</v>
       </c>
@@ -6376,54 +6539,54 @@
       <c r="L28" s="36"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="51">
+      <c r="C29" s="54"/>
+      <c r="D29" s="59">
         <f>D26*E26 + D27*E27</f>
         <v>500</v>
       </c>
-      <c r="E29" s="51"/>
-      <c r="I29" s="44" t="s">
+      <c r="E29" s="59"/>
+      <c r="I29" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="44"/>
-      <c r="K29" s="52">
+      <c r="J29" s="56"/>
+      <c r="K29" s="57">
         <f>K26*L26+K27*L27</f>
         <v>950</v>
       </c>
-      <c r="L29" s="44"/>
+      <c r="L29" s="56"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="I32" s="55" t="s">
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="I32" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="55"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="49"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I34" s="50" t="s">
+      <c r="I34" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="J34" s="50"/>
+      <c r="J34" s="51"/>
       <c r="K34" s="5" t="s">
         <v>1</v>
       </c>
@@ -6432,20 +6595,20 @@
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="54"/>
+      <c r="C35" s="58"/>
       <c r="D35" s="4">
         <v>30</v>
       </c>
       <c r="E35" s="35">
         <v>6</v>
       </c>
-      <c r="I35" s="54" t="s">
+      <c r="I35" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="J35" s="54"/>
+      <c r="J35" s="58"/>
       <c r="K35" s="4">
         <v>30</v>
       </c>
@@ -6454,20 +6617,20 @@
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="54"/>
+      <c r="C36" s="58"/>
       <c r="D36" s="4">
         <v>20</v>
       </c>
       <c r="E36" s="35">
         <v>15</v>
       </c>
-      <c r="I36" s="54" t="s">
+      <c r="I36" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J36" s="54"/>
+      <c r="J36" s="58"/>
       <c r="K36" s="4">
         <v>20</v>
       </c>
@@ -6479,63 +6642,27 @@
       <c r="L37" s="36"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="42"/>
-      <c r="D38" s="51">
+      <c r="C38" s="54"/>
+      <c r="D38" s="59">
         <f>D35*E35 + D36*E36</f>
         <v>480</v>
       </c>
-      <c r="E38" s="51"/>
-      <c r="I38" s="44" t="s">
+      <c r="E38" s="59"/>
+      <c r="I38" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="J38" s="44"/>
-      <c r="K38" s="52">
+      <c r="J38" s="56"/>
+      <c r="K38" s="57">
         <f>K35*L35+K36*L36</f>
         <v>660</v>
       </c>
-      <c r="L38" s="44"/>
+      <c r="L38" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="I32:L32"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="I16:J16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="I10:J10"/>
@@ -6548,6 +6675,42 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="I32:L32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="I38:J38"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6622,20 +6785,20 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="58"/>
-      <c r="H4" s="59" t="s">
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="73"/>
+      <c r="H4" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="61"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="66"/>
       <c r="O4" s="19" t="s">
         <v>8</v>
       </c>
@@ -6680,10 +6843,10 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
@@ -6693,10 +6856,10 @@
       <c r="F6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="63" t="s">
+      <c r="H6" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
@@ -6708,10 +6871,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="40"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="23">
         <v>30</v>
       </c>
@@ -6722,10 +6885,10 @@
         <f>E7/60</f>
         <v>2</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="41"/>
+      <c r="I7" s="53"/>
       <c r="J7" s="25">
         <v>30</v>
       </c>
@@ -6738,10 +6901,10 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="23">
         <v>20</v>
       </c>
@@ -6752,10 +6915,10 @@
         <f>E8/60</f>
         <v>4</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="41"/>
+      <c r="I8" s="53"/>
       <c r="J8" s="25">
         <v>20</v>
       </c>
@@ -6774,43 +6937,43 @@
       <c r="L9" s="29"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66">
+      <c r="C10" s="69"/>
+      <c r="D10" s="74">
         <f>D7*F7+D8*F8</f>
         <v>140</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="67"/>
-      <c r="H10" s="68" t="s">
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
+      <c r="H10" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="69"/>
-      <c r="J10" s="70">
+      <c r="I10" s="79"/>
+      <c r="J10" s="62">
         <f>J7*L7+J8*L8</f>
         <v>152.33333333333334</v>
       </c>
-      <c r="K10" s="70"/>
-      <c r="L10" s="71"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="63"/>
     </row>
     <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="58"/>
-      <c r="H12" s="59" t="s">
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="H12" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="61"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="66"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
@@ -6819,10 +6982,10 @@
       <c r="L13" s="29"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
@@ -6832,10 +6995,10 @@
       <c r="F14" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="63" t="s">
+      <c r="H14" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="50"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
@@ -6847,10 +7010,10 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="23">
         <v>30</v>
       </c>
@@ -6861,10 +7024,10 @@
         <f>E15/60</f>
         <v>4</v>
       </c>
-      <c r="H15" s="73" t="s">
+      <c r="H15" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="41"/>
+      <c r="I15" s="53"/>
       <c r="J15" s="25">
         <v>30</v>
       </c>
@@ -6877,10 +7040,10 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="23">
         <v>20</v>
       </c>
@@ -6891,10 +7054,10 @@
         <f>E16/60</f>
         <v>16</v>
       </c>
-      <c r="H16" s="73" t="s">
+      <c r="H16" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="41"/>
+      <c r="I16" s="53"/>
       <c r="J16" s="25">
         <v>20</v>
       </c>
@@ -6913,26 +7076,26 @@
       <c r="L17" s="29"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66">
+      <c r="C18" s="69"/>
+      <c r="D18" s="74">
         <f>D15*F15+D16*F16</f>
         <v>440</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="67"/>
-      <c r="H18" s="68" t="s">
+      <c r="E18" s="74"/>
+      <c r="F18" s="75"/>
+      <c r="H18" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="69"/>
-      <c r="J18" s="70">
+      <c r="I18" s="79"/>
+      <c r="J18" s="62">
         <f>J15*L15+J16*L16</f>
         <v>609.16666666666674</v>
       </c>
-      <c r="K18" s="70"/>
-      <c r="L18" s="71"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="63"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -6954,6 +7117,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="B8:C8"/>
@@ -6966,18 +7141,6 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>